<commit_message>
add updated project calendar
</commit_message>
<xml_diff>
--- a/DP4_ProjectCalendar.xlsx
+++ b/DP4_ProjectCalendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/candaurn/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE9419A-ED15-A349-82B0-95B116854994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF6F27D-3A68-854D-A534-DBFD942CF308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="38400" windowHeight="21600" xr2:uid="{D0652821-C6A4-458E-81BF-BBA945BD5C25}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" activeTab="3" xr2:uid="{D0652821-C6A4-458E-81BF-BBA945BD5C25}"/>
   </bookViews>
   <sheets>
     <sheet name="SAP GDM&amp;PE" sheetId="1" r:id="rId1"/>
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB52F45-E26E-4881-99AB-9DDABDFB6CBA}">
   <dimension ref="A1:DN28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="111" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="111" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2345,13 +2345,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="13">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D8" s="14">
         <v>44984</v>
       </c>
       <c r="E8" s="18">
-        <v>45002</v>
+        <v>45055</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="3"/>
@@ -4165,13 +4165,13 @@
         <v>13</v>
       </c>
       <c r="C22" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="14">
         <v>44991</v>
       </c>
       <c r="E22" s="18">
-        <v>45023</v>
+        <v>45055</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="3"/>
@@ -5059,6 +5059,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="CT4:CZ4"/>
     <mergeCell ref="DA4:DG4"/>
@@ -5069,12 +5075,6 @@
     <mergeCell ref="BR4:BX4"/>
     <mergeCell ref="BY4:CE4"/>
     <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
   </mergeCells>
   <conditionalFormatting sqref="O22 O9 O11 P7:DN27 G7:N27">
     <cfRule type="expression" dxfId="15" priority="30">
@@ -5173,7 +5173,7 @@
   <dimension ref="A1:DN28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6421,13 +6421,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="13">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D8" s="14">
         <v>44984</v>
       </c>
       <c r="E8" s="18">
-        <v>45002</v>
+        <v>45055</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="3"/>
@@ -8241,7 +8241,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="14">
         <v>44991</v>
@@ -9145,6 +9145,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="CT4:CZ4"/>
     <mergeCell ref="DA4:DG4"/>
@@ -9155,12 +9161,6 @@
     <mergeCell ref="BR4:BX4"/>
     <mergeCell ref="BY4:CE4"/>
     <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
   </mergeCells>
   <conditionalFormatting sqref="O24:O25 O28 O11 P7:DN28 G7:N28 O19:O22">
     <cfRule type="expression" dxfId="11" priority="9">
@@ -12855,6 +12855,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="CT4:CZ4"/>
     <mergeCell ref="DA4:DG4"/>
@@ -12865,12 +12871,6 @@
     <mergeCell ref="BR4:BX4"/>
     <mergeCell ref="BY4:CE4"/>
     <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
   </mergeCells>
   <conditionalFormatting sqref="O15:O16 O11 O24 P7:DN24 G7:N24 O19:O22">
     <cfRule type="expression" dxfId="8" priority="9">
@@ -12968,7 +12968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C84BD7-F5AB-A247-9D22-513879D8F734}">
   <dimension ref="A1:DN25"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -16539,6 +16539,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
     <mergeCell ref="CM4:CS4"/>
     <mergeCell ref="CT4:CZ4"/>
     <mergeCell ref="DA4:DG4"/>
@@ -16549,12 +16555,6 @@
     <mergeCell ref="BR4:BX4"/>
     <mergeCell ref="BY4:CE4"/>
     <mergeCell ref="CF4:CL4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="G4:M4"/>
-    <mergeCell ref="N4:T4"/>
-    <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
   </mergeCells>
   <conditionalFormatting sqref="O15:O16 O11 O22 O24 P8:DN24 G8:N24">
     <cfRule type="expression" dxfId="4" priority="4">

</xml_diff>